<commit_message>
Tool 2 combined Concentration and Mass trends.
</commit_message>
<xml_diff>
--- a/data/data_template.xlsx
+++ b/data/data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpodzorski\Documents\00_gsi_workfiles\5648_TA2\5648_TA2-Transition-Assessment-Assistant_1a\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F886848-3EFB-42A9-97D1-8ABDCB16573C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E34FFD-0D4F-408B-915A-D448A85517C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FFC3D5E4-80F1-4B17-B001-9ABFF7A9C093}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FFC3D5E4-80F1-4B17-B001-9ABFF7A9C093}"/>
   </bookViews>
   <sheets>
     <sheet name="Read_Me" sheetId="3" r:id="rId1"/>
@@ -161,10 +161,10 @@
     <t>Well Grouping</t>
   </si>
   <si>
-    <t>Downstream</t>
-  </si>
-  <si>
     <t>Plume</t>
+  </si>
+  <si>
+    <t>Downgradient</t>
   </si>
 </sst>
 </file>
@@ -172,8 +172,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0000000"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -313,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,21 +333,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,38 +715,38 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -851,7 +856,7 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>40970</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -883,33 +888,33 @@
       <c r="M3" s="1">
         <v>7</v>
       </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>41152.5</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -941,33 +946,33 @@
       <c r="M4" s="1">
         <v>8.49</v>
       </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="10"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>41335</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -999,33 +1004,33 @@
       <c r="M5" s="1">
         <v>10.7</v>
       </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>41517.5</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1057,33 +1062,33 @@
       <c r="M6" s="1">
         <v>11.2</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>41700</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -1111,33 +1116,33 @@
         <v>11.5</v>
       </c>
       <c r="M7" s="1"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="11"/>
-      <c r="AG7" s="11"/>
-      <c r="AH7" s="11"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>41882.5</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -1169,33 +1174,33 @@
       <c r="M8" s="1">
         <v>12</v>
       </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="11"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>42065</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1219,33 +1224,33 @@
       <c r="M9" s="1">
         <v>15</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11"/>
-      <c r="AH9" s="11"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>42247.5</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -1281,33 +1286,33 @@
       <c r="M10" s="1">
         <v>9.4</v>
       </c>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11"/>
-      <c r="AH10" s="11"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="10"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>42430</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -1339,33 +1344,33 @@
         <v>1.85</v>
       </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="11"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="10"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>42612.5</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -1391,33 +1396,33 @@
       <c r="M12" s="1">
         <v>11.6</v>
       </c>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="10"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>42795</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -1451,33 +1456,33 @@
       <c r="M13" s="1">
         <v>14.3</v>
       </c>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+      <c r="AH13" s="10"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>42977.5</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1507,33 +1512,33 @@
         <v>41.9</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="10"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+      <c r="AH14" s="10"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>43160</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1565,33 +1570,33 @@
         <v>13</v>
       </c>
       <c r="M15" s="1"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="10"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
+      <c r="AH15" s="10"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>43342.5</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -1623,33 +1628,33 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="10"/>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="10"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>43525</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -1679,33 +1684,33 @@
         <v>11.5</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>43707.5</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1735,33 +1740,33 @@
         <v>5</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="11"/>
-      <c r="AD18" s="11"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="11"/>
-      <c r="AH18" s="11"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="10"/>
+      <c r="AH18" s="10"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>17</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>43890</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -1783,33 +1788,33 @@
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
-      <c r="AC19" s="11"/>
-      <c r="AD19" s="11"/>
-      <c r="AE19" s="11"/>
-      <c r="AF19" s="11"/>
-      <c r="AG19" s="11"/>
-      <c r="AH19" s="11"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
+      <c r="AH19" s="10"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>44072.5</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -1839,33 +1844,33 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M20" s="1"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="11"/>
-      <c r="AB20" s="11"/>
-      <c r="AC20" s="11"/>
-      <c r="AD20" s="11"/>
-      <c r="AE20" s="11"/>
-      <c r="AF20" s="11"/>
-      <c r="AG20" s="11"/>
-      <c r="AH20" s="11"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="10"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>19</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>44255</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -1893,33 +1898,33 @@
         <v>1.85</v>
       </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-      <c r="AA21" s="11"/>
-      <c r="AB21" s="11"/>
-      <c r="AC21" s="11"/>
-      <c r="AD21" s="11"/>
-      <c r="AE21" s="11"/>
-      <c r="AF21" s="11"/>
-      <c r="AG21" s="11"/>
-      <c r="AH21" s="11"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="10"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>20</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>44437.5</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -1937,27 +1942,27 @@
       <c r="K22" s="2"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
-      <c r="AD22" s="11"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1971,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186B9F43-56CE-4B47-B5C5-CA3BDB0A7AFE}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1985,7 +1990,7 @@
     <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -1995,148 +2000,154 @@
       <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9">
-        <v>53.479223519999998</v>
-      </c>
-      <c r="C2" s="9">
-        <v>-31.637000400000002</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="12">
+        <v>29.731482100000001</v>
+      </c>
+      <c r="C2" s="12">
+        <v>-95.413219999999995</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
-        <v>53.489223520000003</v>
-      </c>
-      <c r="C3" s="9">
-        <v>-31.6470004</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="8">
+        <v>29.740480000000002</v>
+      </c>
+      <c r="C3" s="17">
+        <v>-95.522620000000003</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
-        <v>53.499223520000001</v>
-      </c>
-      <c r="C4" s="9">
-        <v>-31.657000400000001</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="B4" s="8">
+        <v>29.771329999999999</v>
+      </c>
+      <c r="C4" s="8">
+        <v>-95.322329999999994</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9">
-        <v>53.509223519999999</v>
-      </c>
-      <c r="C5" s="9">
-        <v>-31.667000399999999</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="B5" s="8">
+        <v>29.771750000000001</v>
+      </c>
+      <c r="C5" s="8">
+        <v>-95.304130000000001</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
-        <v>53.519223519999997</v>
-      </c>
-      <c r="C6" s="9">
-        <v>-31.677000400000001</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="B6" s="8">
+        <v>29.663129999999999</v>
+      </c>
+      <c r="C6" s="8">
+        <v>-95.326700000000002</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
-        <v>53.529223520000002</v>
-      </c>
-      <c r="C7" s="9">
-        <v>-31.687000399999999</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="B7" s="8">
+        <v>29.74822</v>
+      </c>
+      <c r="C7" s="8">
+        <v>-95.503879999999995</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
-        <v>53.53922352</v>
-      </c>
-      <c r="C8" s="9">
-        <v>-31.6970004</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="8">
+        <v>29.741309999999999</v>
+      </c>
+      <c r="C8" s="8">
+        <v>-95.402460000000005</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
-        <v>53.549223519999998</v>
-      </c>
-      <c r="C9" s="9">
-        <v>-31.707000399999998</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="B9" s="8">
+        <v>29.729009999999999</v>
+      </c>
+      <c r="C9" s="8">
+        <v>-95.433809999999994</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
-        <v>53.559223520000003</v>
-      </c>
-      <c r="C10" s="9">
-        <v>-31.7170004</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="B10" s="8">
+        <v>29.67681</v>
+      </c>
+      <c r="C10" s="8">
+        <v>-95.475409999999997</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K19" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B10">
+  <conditionalFormatting sqref="B2">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;&gt;$E2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C10">
+  <conditionalFormatting sqref="C2">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>#REF!&lt;&gt;$E2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Tools 1 and 2
</commit_message>
<xml_diff>
--- a/data/data_template.xlsx
+++ b/data/data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpodzorski\Documents\00_gsi_workfiles\5648_TA2\5648_TA2-Transition-Assessment-Assistant_1a\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E34FFD-0D4F-408B-915A-D448A85517C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C962642-5E99-49E3-AA57-283307A32F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FFC3D5E4-80F1-4B17-B001-9ABFF7A9C093}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FFC3D5E4-80F1-4B17-B001-9ABFF7A9C093}"/>
   </bookViews>
   <sheets>
     <sheet name="Read_Me" sheetId="3" r:id="rId1"/>
@@ -342,15 +342,15 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -700,7 +700,7 @@
   <dimension ref="A1:AH22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="I3" sqref="I3:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,38 +715,38 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -886,7 +886,7 @@
         <v>37.1</v>
       </c>
       <c r="M3" s="1">
-        <v>7</v>
+        <v>37.1</v>
       </c>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
@@ -944,7 +944,7 @@
         <v>41.9</v>
       </c>
       <c r="M4" s="1">
-        <v>8.49</v>
+        <v>41.9</v>
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
@@ -1002,7 +1002,7 @@
         <v>13</v>
       </c>
       <c r="M5" s="1">
-        <v>10.7</v>
+        <v>13</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
@@ -1060,7 +1060,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="M6" s="1">
-        <v>11.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
@@ -1115,7 +1115,9 @@
       <c r="L7" s="1">
         <v>11.5</v>
       </c>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1">
+        <v>11.5</v>
+      </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
@@ -1172,7 +1174,7 @@
         <v>5</v>
       </c>
       <c r="M8" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
@@ -1221,9 +1223,7 @@
         <v>7</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1">
-        <v>15</v>
-      </c>
+      <c r="M9" s="1"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
@@ -1284,7 +1284,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M10" s="1">
-        <v>9.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -1343,7 +1343,9 @@
       <c r="L11" s="1">
         <v>1.85</v>
       </c>
-      <c r="M11" s="1"/>
+      <c r="M11" s="1">
+        <v>1.85</v>
+      </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -1393,9 +1395,7 @@
         <v>11.2</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1">
-        <v>11.6</v>
-      </c>
+      <c r="M12" s="1"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
@@ -1454,7 +1454,7 @@
         <v>37.1</v>
       </c>
       <c r="M13" s="1">
-        <v>14.3</v>
+        <v>1.8</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1511,7 +1511,9 @@
       <c r="L14" s="1">
         <v>41.9</v>
       </c>
-      <c r="M14" s="1"/>
+      <c r="M14" s="1">
+        <v>1.2</v>
+      </c>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
@@ -1569,7 +1571,9 @@
       <c r="L15" s="1">
         <v>13</v>
       </c>
-      <c r="M15" s="1"/>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
@@ -1627,7 +1631,9 @@
       <c r="L16" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M16" s="1"/>
+      <c r="M16" s="1">
+        <v>1.2</v>
+      </c>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
@@ -1683,7 +1689,9 @@
       <c r="L17" s="1">
         <v>11.5</v>
       </c>
-      <c r="M17" s="1"/>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
@@ -1739,7 +1747,9 @@
       <c r="L18" s="1">
         <v>5</v>
       </c>
-      <c r="M18" s="1"/>
+      <c r="M18" s="1">
+        <v>0.8</v>
+      </c>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
@@ -1843,7 +1853,9 @@
       <c r="L20" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="M20" s="1"/>
+      <c r="M20" s="1">
+        <v>0.7</v>
+      </c>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
@@ -1897,7 +1909,9 @@
       <c r="L21" s="1">
         <v>1.85</v>
       </c>
-      <c r="M21" s="1"/>
+      <c r="M21" s="1">
+        <v>0.5</v>
+      </c>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
@@ -1941,7 +1955,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="M22" s="2"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
@@ -1979,7 +1993,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2009,10 +2023,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="12">
-        <v>29.731482100000001</v>
+        <v>29.731660000000002</v>
       </c>
       <c r="C2" s="12">
-        <v>-95.413219999999995</v>
+        <v>-95.412599999999998</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>41</v>
@@ -2023,10 +2037,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="8">
-        <v>29.740480000000002</v>
-      </c>
-      <c r="C3" s="17">
-        <v>-95.522620000000003</v>
+        <v>29.732970000000002</v>
+      </c>
+      <c r="C3" s="15">
+        <v>-95.413979999999995</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>42</v>
@@ -2037,10 +2051,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8">
-        <v>29.771329999999999</v>
+        <v>29.733080000000001</v>
       </c>
       <c r="C4" s="8">
-        <v>-95.322329999999994</v>
+        <v>-95.413020000000003</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>41</v>
@@ -2051,10 +2065,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8">
-        <v>29.771750000000001</v>
+        <v>29.732679999999998</v>
       </c>
       <c r="C5" s="8">
-        <v>-95.304130000000001</v>
+        <v>-95.411810000000003</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>41</v>
@@ -2065,26 +2079,26 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>29.663129999999999</v>
+        <v>29.733730000000001</v>
       </c>
       <c r="C6" s="8">
-        <v>-95.326700000000002</v>
+        <v>-95.412239999999997</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="8">
-        <v>29.74822</v>
+        <v>29.733250000000002</v>
       </c>
       <c r="C7" s="8">
-        <v>-95.503879999999995</v>
+        <v>-95.411389999999997</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>42</v>
@@ -2095,10 +2109,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8">
-        <v>29.741309999999999</v>
+        <v>29.733989999999999</v>
       </c>
       <c r="C8" s="8">
-        <v>-95.402460000000005</v>
+        <v>-95.410929999999993</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>41</v>
@@ -2109,10 +2123,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8">
-        <v>29.729009999999999</v>
+        <v>29.732690000000002</v>
       </c>
       <c r="C9" s="8">
-        <v>-95.433809999999994</v>
+        <v>-95.413179999999997</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>42</v>
@@ -2123,17 +2137,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="8">
-        <v>29.67681</v>
+        <v>29.732559999999999</v>
       </c>
       <c r="C10" s="8">
-        <v>-95.475409999999997</v>
+        <v>-95.412350000000004</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K19" s="16"/>
+      <c r="K19" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
2022-02-25 Borden Tool update
</commit_message>
<xml_diff>
--- a/data/data_template.xlsx
+++ b/data/data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpodzorski\Documents\00_gsi_workfiles\5648_TA2\5648_TA2-Transition-Assessment-Assistant_1a\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmori\Desktop\GSI Work Files\5648_SERDP_Borden\5648_TA2_Transition_Assessment_Assistant_20210802\5648_TA2-Transition-Assessment-Assistant_1a\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E34FFD-0D4F-408B-915A-D448A85517C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF772090-3B9C-484B-A13A-546566488C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FFC3D5E4-80F1-4B17-B001-9ABFF7A9C093}"/>
+    <workbookView xWindow="29565" yWindow="930" windowWidth="15975" windowHeight="15120" activeTab="2" xr2:uid="{FFC3D5E4-80F1-4B17-B001-9ABFF7A9C093}"/>
   </bookViews>
   <sheets>
     <sheet name="Read_Me" sheetId="3" r:id="rId1"/>
@@ -342,15 +342,15 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,7 +689,7 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -700,55 +700,55 @@
   <dimension ref="A1:AH22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="I3" sqref="I3:I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -852,7 +852,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -886,7 +886,7 @@
         <v>37.1</v>
       </c>
       <c r="M3" s="1">
-        <v>7</v>
+        <v>37.1</v>
       </c>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
@@ -910,7 +910,7 @@
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -944,7 +944,7 @@
         <v>41.9</v>
       </c>
       <c r="M4" s="1">
-        <v>8.49</v>
+        <v>41.9</v>
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
@@ -968,7 +968,7 @@
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>13</v>
       </c>
       <c r="M5" s="1">
-        <v>10.7</v>
+        <v>13</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
@@ -1026,7 +1026,7 @@
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="M6" s="1">
-        <v>11.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
@@ -1084,7 +1084,7 @@
       <c r="AG6" s="10"/>
       <c r="AH6" s="10"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -1115,7 +1115,9 @@
       <c r="L7" s="1">
         <v>11.5</v>
       </c>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1">
+        <v>11.5</v>
+      </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
@@ -1138,7 +1140,7 @@
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -1172,7 +1174,7 @@
         <v>5</v>
       </c>
       <c r="M8" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
@@ -1196,7 +1198,7 @@
       <c r="AG8" s="10"/>
       <c r="AH8" s="10"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -1221,9 +1223,7 @@
         <v>7</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1">
-        <v>15</v>
-      </c>
+      <c r="M9" s="1"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
@@ -1246,7 +1246,7 @@
       <c r="AG9" s="10"/>
       <c r="AH9" s="10"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="M10" s="1">
-        <v>9.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -1308,7 +1308,7 @@
       <c r="AG10" s="10"/>
       <c r="AH10" s="10"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -1343,7 +1343,9 @@
       <c r="L11" s="1">
         <v>1.85</v>
       </c>
-      <c r="M11" s="1"/>
+      <c r="M11" s="1">
+        <v>1.85</v>
+      </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -1366,7 +1368,7 @@
       <c r="AG11" s="10"/>
       <c r="AH11" s="10"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -1393,9 +1395,7 @@
         <v>11.2</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1">
-        <v>11.6</v>
-      </c>
+      <c r="M12" s="1"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
@@ -1418,7 +1418,7 @@
       <c r="AG12" s="10"/>
       <c r="AH12" s="10"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>37.1</v>
       </c>
       <c r="M13" s="1">
-        <v>14.3</v>
+        <v>1.8</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1478,7 +1478,7 @@
       <c r="AG13" s="10"/>
       <c r="AH13" s="10"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -1511,7 +1511,9 @@
       <c r="L14" s="1">
         <v>41.9</v>
       </c>
-      <c r="M14" s="1"/>
+      <c r="M14" s="1">
+        <v>1.2</v>
+      </c>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
@@ -1534,7 +1536,7 @@
       <c r="AG14" s="10"/>
       <c r="AH14" s="10"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -1569,7 +1571,9 @@
       <c r="L15" s="1">
         <v>13</v>
       </c>
-      <c r="M15" s="1"/>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
@@ -1592,7 +1596,7 @@
       <c r="AG15" s="10"/>
       <c r="AH15" s="10"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -1627,7 +1631,9 @@
       <c r="L16" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M16" s="1"/>
+      <c r="M16" s="1">
+        <v>1.2</v>
+      </c>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
@@ -1650,7 +1656,7 @@
       <c r="AG16" s="10"/>
       <c r="AH16" s="10"/>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -1683,7 +1689,9 @@
       <c r="L17" s="1">
         <v>11.5</v>
       </c>
-      <c r="M17" s="1"/>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
@@ -1706,7 +1714,7 @@
       <c r="AG17" s="10"/>
       <c r="AH17" s="10"/>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>16</v>
       </c>
@@ -1739,7 +1747,9 @@
       <c r="L18" s="1">
         <v>5</v>
       </c>
-      <c r="M18" s="1"/>
+      <c r="M18" s="1">
+        <v>0.8</v>
+      </c>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
@@ -1762,7 +1772,7 @@
       <c r="AG18" s="10"/>
       <c r="AH18" s="10"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -1810,7 +1820,7 @@
       <c r="AG19" s="10"/>
       <c r="AH19" s="10"/>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -1843,7 +1853,9 @@
       <c r="L20" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="M20" s="1"/>
+      <c r="M20" s="1">
+        <v>0.7</v>
+      </c>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
@@ -1866,7 +1878,7 @@
       <c r="AG20" s="10"/>
       <c r="AH20" s="10"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -1897,7 +1909,9 @@
       <c r="L21" s="1">
         <v>1.85</v>
       </c>
-      <c r="M21" s="1"/>
+      <c r="M21" s="1">
+        <v>0.5</v>
+      </c>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
@@ -1920,7 +1934,7 @@
       <c r="AG21" s="10"/>
       <c r="AH21" s="10"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -1941,7 +1955,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="M22" s="2"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
@@ -1979,18 +1993,18 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -2004,136 +2018,136 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="12">
-        <v>29.731482100000001</v>
+        <v>29.731660000000002</v>
       </c>
       <c r="C2" s="12">
-        <v>-95.413219999999995</v>
+        <v>-95.412599999999998</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8">
-        <v>29.740480000000002</v>
-      </c>
-      <c r="C3" s="17">
-        <v>-95.522620000000003</v>
+        <v>29.732970000000002</v>
+      </c>
+      <c r="C3" s="15">
+        <v>-95.413979999999995</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="8">
-        <v>29.771329999999999</v>
+        <v>29.733080000000001</v>
       </c>
       <c r="C4" s="8">
-        <v>-95.322329999999994</v>
+        <v>-95.413020000000003</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="8">
-        <v>29.771750000000001</v>
+        <v>29.732679999999998</v>
       </c>
       <c r="C5" s="8">
-        <v>-95.304130000000001</v>
+        <v>-95.411810000000003</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <v>29.663129999999999</v>
+        <v>29.733730000000001</v>
       </c>
       <c r="C6" s="8">
-        <v>-95.326700000000002</v>
+        <v>-95.412239999999997</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="8">
-        <v>29.74822</v>
+        <v>29.733250000000002</v>
       </c>
       <c r="C7" s="8">
-        <v>-95.503879999999995</v>
+        <v>-95.411389999999997</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="8">
-        <v>29.741309999999999</v>
+        <v>29.733989999999999</v>
       </c>
       <c r="C8" s="8">
-        <v>-95.402460000000005</v>
+        <v>-95.410929999999993</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="8">
-        <v>29.729009999999999</v>
+        <v>29.732690000000002</v>
       </c>
       <c r="C9" s="8">
-        <v>-95.433809999999994</v>
+        <v>-95.413179999999997</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="8">
-        <v>29.67681</v>
+        <v>29.732559999999999</v>
       </c>
       <c r="C10" s="8">
-        <v>-95.475409999999997</v>
+        <v>-95.412350000000004</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K19" s="16"/>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>